<commit_message>
Use specific name for GCS URI instead of file_location
</commit_message>
<xml_diff>
--- a/template_examples/misc_data_template.xlsx
+++ b/template_examples/misc_data_template.xlsx
@@ -65,7 +65,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a user's computer.</t>
+          <t xml:space="preserve">An optional (short) name of the file</t>
         </r>
       </text>
     </comment>
@@ -79,7 +79,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">An optional (short) name of the file</t>
+          <t xml:space="preserve">Path to a file on a user's computer.</t>
         </r>
       </text>
     </comment>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="37">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -134,10 +134,10 @@
     <t xml:space="preserve">#header</t>
   </si>
   <si>
-    <t xml:space="preserve">File location</t>
+    <t xml:space="preserve">File name</t>
   </si>
   <si>
-    <t xml:space="preserve">File name</t>
+    <t xml:space="preserve">File location</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -146,19 +146,28 @@
     <t xml:space="preserve">#data</t>
   </si>
   <si>
+    <t xml:space="preserve">foo.txt</t>
+  </si>
+  <si>
     <t xml:space="preserve">foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file_name.txt</t>
   </si>
   <si>
     <t xml:space="preserve">bar</t>
   </si>
   <si>
-    <t xml:space="preserve">file_name</t>
+    <t xml:space="preserve">baz.txt</t>
   </si>
   <si>
     <t xml:space="preserve">baz</t>
   </si>
   <si>
     <t xml:space="preserve">this is a description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file_name.barbaz</t>
   </si>
   <si>
     <t xml:space="preserve">barbaz</t>
@@ -188,10 +197,10 @@
     <t xml:space="preserve">Section 'Files' of tab 'Misc'</t>
   </si>
   <si>
-    <t xml:space="preserve">Path to a file on a user's computer.</t>
+    <t xml:space="preserve">An optional (short) name of the file</t>
   </si>
   <si>
-    <t xml:space="preserve">An optional (short) name of the file</t>
+    <t xml:space="preserve">Path to a file on a user's computer.</t>
   </si>
   <si>
     <t xml:space="preserve">An optional long string describing the file, its purpose, and/or its content.</t>
@@ -438,10 +447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2006"/>
+  <dimension ref="A1:E2006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -504,48 +513,57 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>19</v>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10568,12 +10586,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10581,10 +10599,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10592,18 +10610,18 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10611,10 +10629,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10622,10 +10640,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10633,10 +10651,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -10679,17 +10697,17 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>